<commit_message>
Update for lockdown feature
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HelloWorld\covid-shanghai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED70210-B395-4843-AD5D-DC5C65419AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B8305-8748-416D-B4DA-37530A8D43AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3630" windowWidth="21600" windowHeight="11385" xr2:uid="{0A12BC7F-B800-4DBA-AB55-EF7624A060F3}"/>
+    <workbookView xWindow="8385" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{0A12BC7F-B800-4DBA-AB55-EF7624A060F3}"/>
   </bookViews>
   <sheets>
     <sheet name="拟合" sheetId="3" r:id="rId1"/>
@@ -1836,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10553464-E8C6-4D82-A638-DDD6CC6B08F7}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3394,6 +3394,44 @@
       <c r="J41" s="2">
         <f t="shared" si="42"/>
         <v>0.1529410956645969</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44661</v>
+      </c>
+      <c r="B42" s="4">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>914</v>
+      </c>
+      <c r="D42">
+        <v>25173</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42" si="43">D42+C42</f>
+        <v>26087</v>
+      </c>
+      <c r="F42" s="2">
+        <f>E42/E41-1</f>
+        <v>4.5864571222387074E-2</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ref="G42" si="44">SUM(C29:C42)</f>
+        <v>6918</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42" si="45">SUM(D29:D42)</f>
+        <v>183528</v>
+      </c>
+      <c r="I42">
+        <f t="shared" ref="I42" si="46">SUM(E29:E42)</f>
+        <v>190446</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" ref="J42" si="47">I42/I41-1</f>
+        <v>0.13455936232194876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix 20220416 data bug
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HelloWorld\covid-shanghai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C76DE-8F2D-4D5C-865F-7C63B77F1967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462D60D-7680-4764-A7AF-B2BEEBD3FACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A12BC7F-B800-4DBA-AB55-EF7624A060F3}"/>
   </bookViews>
@@ -300,7 +300,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.24386990318572185"/>
+          <c:x val="0.23884774571696307"/>
           <c:y val="3.3553138010997838E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -477,10 +477,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>拟合!$B$2:$B$45</c:f>
+              <c:f>拟合!$B$2:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -612,16 +612,25 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>拟合!$E$2:$E$45</c:f>
+              <c:f>拟合!$E$2:$E$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -753,6 +762,15 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>27719</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>23072</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>23513</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>24820</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1528,14 +1546,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>128307</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>5043</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>638734</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1860,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10553464-E8C6-4D82-A638-DDD6CC6B08F7}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C1:C1048576"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3646,6 +3664,44 @@
       <c r="J47" s="2">
         <f t="shared" si="53"/>
         <v>6.3641576795723243E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44667</v>
+      </c>
+      <c r="B48" s="4">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>3238</v>
+      </c>
+      <c r="D48">
+        <v>21582</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48" si="54">D48+C48</f>
+        <v>24820</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" ref="F48" si="55">E48/E47-1</f>
+        <v>5.558627142431849E-2</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ref="G48" si="56">SUM(C35:C48)</f>
+        <v>19869</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48" si="57">SUM(D35:D48)</f>
+        <v>284222</v>
+      </c>
+      <c r="I48">
+        <f t="shared" ref="I48" si="58">SUM(E35:E48)</f>
+        <v>304091</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" ref="J48" si="59">I48/I47-1</f>
+        <v>5.7718863153354727E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>